<commit_message>
added added source data, added youngs_moduli
</commit_message>
<xml_diff>
--- a/Messungen/Neuer Ordner/DMA_BoseRolauffs_2020-12-22.xlsx
+++ b/Messungen/Neuer Ordner/DMA_BoseRolauffs_2020-12-22.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annar\Documents\Backup ZBSA Aug 2019\02_Labor\01_Laborbuch\Protokolle\2020_Q4\DMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_RESEARCH\08_Dynamic Mechanical Analysis\Messungen\Neuer Ordner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5672A0AE-E39B-4ED1-9B24-54A019520AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F6A6B7-42C9-4D98-92D3-AE887576D575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{CFE59A7A-123F-4CFB-8640-2D9BC7AAE474}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{CFE59A7A-123F-4CFB-8640-2D9BC7AAE474}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle2 (2)" sheetId="3" r:id="rId3"/>
-    <sheet name="Tabelle2 (3)" sheetId="4" r:id="rId4"/>
+    <sheet name="Geometrie" sheetId="5" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
+    <sheet name="Tabelle2 (2)" sheetId="3" r:id="rId4"/>
+    <sheet name="Tabelle2 (3)" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="99">
   <si>
     <t>Protein</t>
   </si>
@@ -330,6 +331,9 @@
   </si>
   <si>
     <t>initial</t>
+  </si>
+  <si>
+    <t>kept</t>
   </si>
 </sst>
 </file>
@@ -16696,8 +16700,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17907,6 +17911,941 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8C8029-9ECF-4FDD-91DF-BAEC4E3D5A85}">
+  <dimension ref="A1:F65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="10">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="10">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="6">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="10">
+        <v>3</v>
+      </c>
+      <c r="C38" s="10">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="1">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1">
+        <v>3</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="1">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="1">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1">
+        <v>3</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="6">
+        <v>8</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78937BAA-4D3E-42A9-A748-227AF439B3B1}">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A3:L44"/>
@@ -19159,7 +20098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB35968-46ED-46B0-B808-F6C059FF4A83}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A2:M42"/>
@@ -20109,12 +21048,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0882F0-6C53-4ACC-B2B8-74FD8886BACB}">
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A3:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>

</xml_diff>